<commit_message>
add hinmoku.py livinhouse fab z
</commit_message>
<xml_diff>
--- a/makepo/POH207544(0912_VesselHAKATA_Port).xlsx
+++ b/makepo/POH207544(0912_VesselHAKATA_Port).xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
   <si>
     <t>INOAC INTERNATIONAL CO.,LTD.</t>
   </si>
@@ -285,6 +285,15 @@
   </si>
   <si>
     <t>156166</t>
+  </si>
+  <si>
+    <t>CH1099-3P+0.5P SP/183</t>
+  </si>
+  <si>
+    <t>CH1099-3PSET SP/183</t>
+  </si>
+  <si>
+    <t>156301</t>
   </si>
   <si>
     <t>total</t>
@@ -1284,7 +1293,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
       <selection activeCell="C11" sqref="C11"/>
@@ -1334,7 +1343,7 @@
       </c>
       <c r="I6" s="71" t="n"/>
       <c r="J6" s="72" t="n">
-        <v>43675</v>
+        <v>43676</v>
       </c>
       <c r="K6" s="73" t="n"/>
       <c r="L6" s="73" t="n"/>
@@ -2533,96 +2542,115 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="45" s="30" spans="1:14">
-      <c r="B45" s="31" t="n"/>
-      <c r="C45" s="32" t="n"/>
-      <c r="D45" s="33" t="n"/>
-      <c r="E45" s="32" t="n"/>
-      <c r="F45" s="34" t="n"/>
-      <c r="G45" s="77" t="n"/>
-      <c r="H45" s="36" t="n"/>
+      <c r="B45" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" s="77" t="n">
+        <v>442.5</v>
+      </c>
+      <c r="H45" s="36">
+        <f>E45*G45</f>
+        <v/>
+      </c>
       <c r="I45" s="37" t="n"/>
-      <c r="J45" s="38" t="n"/>
-      <c r="K45" s="78" t="n"/>
-      <c r="L45" s="32" t="n"/>
+      <c r="J45" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="K45" s="78">
+        <f>E45*N45</f>
+        <v/>
+      </c>
+      <c r="L45" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="46" s="30" spans="1:14">
-      <c r="B46" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="E46" s="42">
-        <f>SUM(E16:E45)</f>
-        <v/>
-      </c>
-      <c r="H46" s="43">
-        <f>SUM(H16:H45)</f>
-        <v/>
-      </c>
-      <c r="I46" s="69" t="n"/>
-      <c r="J46" s="45" t="n"/>
-      <c r="K46" s="79">
-        <f>SUM(K16:K45)</f>
-        <v/>
-      </c>
+      <c r="B46" s="31" t="n"/>
+      <c r="C46" s="32" t="n"/>
+      <c r="D46" s="33" t="n"/>
+      <c r="E46" s="32" t="n"/>
+      <c r="F46" s="34" t="n"/>
+      <c r="G46" s="77" t="n"/>
+      <c r="H46" s="36" t="n"/>
+      <c r="I46" s="37" t="n"/>
+      <c r="J46" s="38" t="n"/>
+      <c r="K46" s="78" t="n"/>
+      <c r="L46" s="32" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="47" s="30" spans="1:14">
-      <c r="C47" s="47" t="s">
+      <c r="B47" s="23" t="s">
         <v>84</v>
       </c>
+      <c r="C47" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47" s="42">
+        <f>SUM(E16:E46)</f>
+        <v/>
+      </c>
+      <c r="H47" s="43">
+        <f>SUM(H16:H46)</f>
+        <v/>
+      </c>
+      <c r="I47" s="69" t="n"/>
+      <c r="J47" s="45" t="n"/>
+      <c r="K47" s="79">
+        <f>SUM(K16:K46)</f>
+        <v/>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="48" s="30" spans="1:14">
-      <c r="B48" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="D48" s="50" t="s">
+      <c r="C48" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="80" t="n">
-        <v>43720</v>
-      </c>
-      <c r="I48" s="81" t="n"/>
-      <c r="J48" s="57" t="n"/>
-      <c r="K48" s="57" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="49" s="30" spans="1:14">
       <c r="B49" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="52" t="s">
+      <c r="C49" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="D49" s="48" t="s">
+      <c r="D49" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="E49" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="F49" s="54" t="n"/>
-      <c r="H49" s="68" t="n"/>
+      <c r="E49" s="80" t="n">
+        <v>43720</v>
+      </c>
       <c r="I49" s="81" t="n"/>
       <c r="J49" s="57" t="n"/>
       <c r="K49" s="57" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="50" s="30" spans="1:14">
       <c r="B50" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="C50" s="52" t="s">
+      <c r="D50" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="D50" s="48" t="s">
+      <c r="E50" s="53" t="s">
         <v>94</v>
-      </c>
-      <c r="E50" s="54" t="s">
-        <v>95</v>
       </c>
       <c r="F50" s="54" t="n"/>
       <c r="H50" s="68" t="n"/>
@@ -2632,16 +2660,16 @@
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="51" s="30" spans="1:14">
       <c r="B51" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C51" s="52" t="s">
+      <c r="D51" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="48" t="s">
+      <c r="E51" s="54" t="s">
         <v>98</v>
-      </c>
-      <c r="E51" s="52" t="s">
-        <v>99</v>
       </c>
       <c r="F51" s="54" t="n"/>
       <c r="H51" s="68" t="n"/>
@@ -2650,33 +2678,47 @@
       <c r="K51" s="57" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="52" s="30" spans="1:14">
-      <c r="B52" s="48" t="n"/>
-      <c r="C52" s="54" t="n"/>
-      <c r="D52" s="48" t="n"/>
-      <c r="E52" s="53" t="n"/>
+      <c r="B52" s="48" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" s="52" t="s">
+        <v>102</v>
+      </c>
       <c r="F52" s="54" t="n"/>
+      <c r="H52" s="68" t="n"/>
       <c r="I52" s="81" t="n"/>
+      <c r="J52" s="57" t="n"/>
+      <c r="K52" s="57" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="53" s="30" spans="1:14">
-      <c r="C53" s="56">
+      <c r="B53" s="48" t="n"/>
+      <c r="C53" s="54" t="n"/>
+      <c r="D53" s="48" t="n"/>
+      <c r="E53" s="53" t="n"/>
+      <c r="F53" s="54" t="n"/>
+      <c r="I53" s="81" t="n"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="24" r="54" s="30" spans="1:14">
+      <c r="C54" s="56">
         <f>+B7</f>
         <v/>
       </c>
-      <c r="F53" s="56" t="s">
+      <c r="F54" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="I53" s="81" t="n"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="24" r="54" s="30" spans="1:14">
-      <c r="C54" s="54" t="n"/>
-      <c r="F54" s="54" t="n"/>
       <c r="I54" s="81" t="n"/>
-      <c r="K54" s="57" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="55" s="30" spans="1:14">
       <c r="C55" s="54" t="n"/>
       <c r="F55" s="54" t="n"/>
       <c r="I55" s="81" t="n"/>
+      <c r="K55" s="57" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="56" s="30" spans="1:14">
       <c r="C56" s="54" t="n"/>
@@ -2684,27 +2726,31 @@
       <c r="I56" s="81" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="57" s="30" spans="1:14">
-      <c r="C57" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="F57" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="G57" s="60" t="n"/>
-      <c r="H57" s="82" t="s">
-        <v>102</v>
-      </c>
-      <c r="I57" s="83" t="n"/>
-      <c r="J57" s="63" t="n"/>
+      <c r="C57" s="54" t="n"/>
+      <c r="F57" s="54" t="n"/>
+      <c r="I57" s="81" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" ht="24" r="58" s="30" spans="1:14">
-      <c r="C58" s="54" t="n"/>
-      <c r="F58" s="64" t="s">
+      <c r="C58" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="I58" s="81" t="n"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="24" r="59" s="30" spans="1:14"/>
+      <c r="F58" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="G58" s="60" t="n"/>
+      <c r="H58" s="82" t="s">
+        <v>105</v>
+      </c>
+      <c r="I58" s="83" t="n"/>
+      <c r="J58" s="63" t="n"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="24" r="59" s="30" spans="1:14">
+      <c r="C59" s="54" t="n"/>
+      <c r="F59" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="I59" s="81" t="n"/>
+    </row>
     <row customFormat="1" customHeight="1" ht="24" r="60" s="30" spans="1:14"/>
     <row customFormat="1" customHeight="1" ht="24" r="61" s="30" spans="1:14"/>
     <row customFormat="1" customHeight="1" ht="24" r="62" s="30" spans="1:14"/>
@@ -2963,7 +3009,7 @@
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="E303:G303"/>
-    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E49:H49"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins bottom="0" footer="0.5118110236220472" header="0.5118110236220472" left="0" right="0" top="0"/>

</xml_diff>